<commit_message>
Updated Fp1 file - fixed typo
</commit_message>
<xml_diff>
--- a/data/Behavior data/Fp1_Motor_GI_function.xlsx
+++ b/data/Behavior data/Fp1_Motor_GI_function.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://caltech-my.sharepoint.com/personal/anamois_caltech_edu/Documents/Caltech/MZ Lab/Write ups/Paper/Data availability/Behavior data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="131" documentId="13_ncr:1_{05E175B3-CFDA-3D4D-85F3-9C6F7C234B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF79DF56-88E5-DC44-9871-BEAF7CFA960F}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="13_ncr:1_{05E175B3-CFDA-3D4D-85F3-9C6F7C234B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{03C370FF-DA5E-B54C-BD75-57C686FEF95A}"/>
   <bookViews>
-    <workbookView xWindow="3380" yWindow="1260" windowWidth="27840" windowHeight="22320" activeTab="1" xr2:uid="{8FAD2B0A-511F-8C4E-B0A9-D9067B35B2EF}"/>
+    <workbookView xWindow="25760" yWindow="1700" windowWidth="22660" windowHeight="22320" firstSheet="1" activeTab="10" xr2:uid="{8FAD2B0A-511F-8C4E-B0A9-D9067B35B2EF}"/>
   </bookViews>
   <sheets>
     <sheet name="Beam_time" sheetId="4" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="25">
   <si>
     <t>Genotype</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>ASO</t>
-  </si>
-  <si>
-    <t>Fpr</t>
   </si>
   <si>
     <t>Weight</t>
@@ -203,6 +200,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -505,7 +506,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H46" sqref="H46"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -524,7 +525,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -702,7 +703,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -719,7 +720,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -736,7 +737,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -753,7 +754,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -767,7 +768,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -784,7 +785,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -801,7 +802,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -988,7 +989,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -1005,7 +1006,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -1022,7 +1023,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -1039,7 +1040,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -1056,7 +1057,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -1078,7 +1079,7 @@
   <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="G29" sqref="G29:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1097,13 +1098,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="G1" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -1341,7 +1342,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -1364,7 +1365,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -1387,7 +1388,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -1410,7 +1411,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -1433,7 +1434,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -1456,7 +1457,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -1479,7 +1480,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -1732,7 +1733,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -1755,7 +1756,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -1778,7 +1779,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -1801,7 +1802,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -1824,7 +1825,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -1851,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EBAE04-AF09-154C-9881-0AB2D07A68B9}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H29" sqref="H29:H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1874,13 +1875,13 @@
         <v>3</v>
       </c>
       <c r="F1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="G1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>23</v>
-      </c>
-      <c r="H1" s="8" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.2">
@@ -2151,7 +2152,7 @@
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D12">
         <v>5</v>
@@ -2177,7 +2178,7 @@
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13">
         <v>5</v>
@@ -2203,7 +2204,7 @@
         <v>8</v>
       </c>
       <c r="C14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14">
         <v>5</v>
@@ -2229,7 +2230,7 @@
         <v>8</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15">
         <v>5</v>
@@ -2255,7 +2256,7 @@
         <v>8</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16">
         <v>6</v>
@@ -2281,7 +2282,7 @@
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17">
         <v>6</v>
@@ -2307,7 +2308,7 @@
         <v>8</v>
       </c>
       <c r="C18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18">
         <v>6</v>
@@ -2593,7 +2594,7 @@
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29">
         <v>11</v>
@@ -2619,7 +2620,7 @@
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30">
         <v>11</v>
@@ -2645,7 +2646,7 @@
         <v>8</v>
       </c>
       <c r="C31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31">
         <v>12</v>
@@ -2671,7 +2672,7 @@
         <v>8</v>
       </c>
       <c r="C32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32">
         <v>12</v>
@@ -2697,7 +2698,7 @@
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33">
         <v>12</v>
@@ -2744,7 +2745,7 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2922,7 +2923,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -2939,7 +2940,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -2956,7 +2957,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -2973,7 +2974,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -2990,7 +2991,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -3007,7 +3008,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -3024,7 +3025,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -3211,7 +3212,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -3228,7 +3229,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -3245,7 +3246,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -3262,7 +3263,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -3279,7 +3280,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -3300,8 +3301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FFF1D44-7D0D-854F-880D-8CEEEE9F6597}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G29" sqref="G29:G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3320,13 +3321,13 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
       <c r="G1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
@@ -3564,7 +3565,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -3588,7 +3589,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -3612,7 +3613,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -3636,7 +3637,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -3650,7 +3651,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -3674,7 +3675,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -3698,7 +3699,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -3952,7 +3953,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -3976,7 +3977,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -4000,7 +4001,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -4024,7 +4025,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -4048,7 +4049,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -4077,7 +4078,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:G1048576"/>
+      <selection activeCell="E29" sqref="E29:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4096,7 +4097,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4274,7 +4275,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -4291,7 +4292,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -4308,7 +4309,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -4325,7 +4326,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -4342,7 +4343,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -4359,7 +4360,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -4376,7 +4377,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -4563,7 +4564,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -4580,7 +4581,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -4597,7 +4598,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -4614,7 +4615,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -4631,7 +4632,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -4653,7 +4654,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:B33"/>
+      <selection activeCell="E29" sqref="E29:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4672,7 +4673,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -4850,7 +4851,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -4867,7 +4868,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -4884,7 +4885,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -4901,7 +4902,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -4918,7 +4919,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -4935,7 +4936,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -4952,7 +4953,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -5139,7 +5140,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -5156,7 +5157,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -5173,7 +5174,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -5190,7 +5191,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -5207,7 +5208,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -5229,7 +5230,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="E29" sqref="E29:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5248,7 +5249,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -5426,7 +5427,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -5443,7 +5444,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -5460,7 +5461,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -5477,7 +5478,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -5494,7 +5495,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -5511,7 +5512,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -5528,7 +5529,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -5715,7 +5716,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -5732,7 +5733,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -5749,7 +5750,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -5766,7 +5767,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -5783,7 +5784,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -5805,7 +5806,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="E29" sqref="E29:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5824,7 +5825,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -6002,7 +6003,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -6019,7 +6020,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -6036,7 +6037,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -6053,7 +6054,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -6070,7 +6071,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -6087,7 +6088,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -6104,7 +6105,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -6291,7 +6292,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -6308,7 +6309,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -6325,7 +6326,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -6342,7 +6343,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -6359,7 +6360,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -6381,7 +6382,7 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H1048576"/>
+      <selection activeCell="E29" sqref="E29:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6400,7 +6401,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -6578,7 +6579,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -6595,7 +6596,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -6612,7 +6613,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -6629,7 +6630,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -6646,7 +6647,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -6663,7 +6664,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -6680,7 +6681,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -6867,7 +6868,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -6884,7 +6885,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -6901,7 +6902,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -6918,7 +6919,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -6935,7 +6936,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -6957,7 +6958,7 @@
   <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E29" sqref="E29:E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6976,7 +6977,7 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -7154,7 +7155,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -7171,7 +7172,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -7188,7 +7189,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -7205,7 +7206,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -7222,7 +7223,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -7239,7 +7240,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -7256,7 +7257,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -7443,7 +7444,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -7463,7 +7464,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -7480,7 +7481,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -7497,7 +7498,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -7514,7 +7515,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -7536,7 +7537,7 @@
   <dimension ref="A1:J33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="J29" sqref="J29:J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7555,22 +7556,22 @@
         <v>3</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>20</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -7918,7 +7919,7 @@
         <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="C12">
         <v>5</v>
@@ -7936,11 +7937,11 @@
         <v>1037.4000000000001</v>
       </c>
       <c r="H12">
-        <f>F12-E12</f>
+        <f t="shared" ref="H12:H18" si="2">F12-E12</f>
         <v>30.400000000000091</v>
       </c>
       <c r="I12">
-        <f>G12-E12</f>
+        <f t="shared" ref="I12:I18" si="3">G12-E12</f>
         <v>13.100000000000136</v>
       </c>
       <c r="J12">
@@ -7952,7 +7953,7 @@
         <v>8</v>
       </c>
       <c r="B13" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C13">
         <v>5</v>
@@ -7970,11 +7971,11 @@
         <v>1044.8</v>
       </c>
       <c r="H13">
-        <f>F13-E13</f>
+        <f t="shared" si="2"/>
         <v>44</v>
       </c>
       <c r="I13">
-        <f>G13-E13</f>
+        <f t="shared" si="3"/>
         <v>16.299999999999955</v>
       </c>
       <c r="J13">
@@ -7986,7 +7987,7 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14">
         <v>5</v>
@@ -8004,11 +8005,11 @@
         <v>1033.8</v>
       </c>
       <c r="H14">
-        <f>F14-E14</f>
+        <f t="shared" si="2"/>
         <v>19.700000000000045</v>
       </c>
       <c r="I14">
-        <f>G14-E14</f>
+        <f t="shared" si="3"/>
         <v>7.5999999999999091</v>
       </c>
       <c r="J14">
@@ -8020,7 +8021,7 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15">
         <v>5</v>
@@ -8038,11 +8039,11 @@
         <v>1037</v>
       </c>
       <c r="H15">
-        <f>F15-E15</f>
+        <f t="shared" si="2"/>
         <v>17.799999999999955</v>
       </c>
       <c r="I15">
-        <f>G15-E15</f>
+        <f t="shared" si="3"/>
         <v>11.200000000000045</v>
       </c>
       <c r="J15">
@@ -8054,7 +8055,7 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16">
         <v>6</v>
@@ -8072,11 +8073,11 @@
         <v>1031</v>
       </c>
       <c r="H16">
-        <f>F16-E16</f>
+        <f t="shared" si="2"/>
         <v>20.900000000000091</v>
       </c>
       <c r="I16">
-        <f>G16-E16</f>
+        <f t="shared" si="3"/>
         <v>8.5</v>
       </c>
       <c r="J16">
@@ -8088,7 +8089,7 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17">
         <v>6</v>
@@ -8106,11 +8107,11 @@
         <v>1013.8</v>
       </c>
       <c r="H17">
-        <f>F17-E17</f>
+        <f t="shared" si="2"/>
         <v>25.799999999999955</v>
       </c>
       <c r="I17">
-        <f>G17-E17</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="J17">
@@ -8122,7 +8123,7 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18">
         <v>6</v>
@@ -8140,11 +8141,11 @@
         <v>1040.5999999999999</v>
       </c>
       <c r="H18">
-        <f>F18-E18</f>
+        <f t="shared" si="2"/>
         <v>19.700000000000045</v>
       </c>
       <c r="I18">
-        <f>G18-E18</f>
+        <f t="shared" si="3"/>
         <v>12.399999999999864</v>
       </c>
       <c r="J18">
@@ -8195,7 +8196,7 @@
         <v>978</v>
       </c>
       <c r="H20">
-        <f t="shared" ref="H20:H33" si="2">F20-E20</f>
+        <f t="shared" ref="H20:H33" si="4">F20-E20</f>
         <v>18.400000000000091</v>
       </c>
       <c r="I20">
@@ -8229,11 +8230,11 @@
         <v>947.4</v>
       </c>
       <c r="H21">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>33.399999999999977</v>
       </c>
       <c r="I21">
-        <f t="shared" ref="I21:I33" si="3">G21-E21</f>
+        <f t="shared" ref="I21:I33" si="5">G21-E21</f>
         <v>12.899999999999977</v>
       </c>
       <c r="J21">
@@ -8263,11 +8264,11 @@
         <v>984.9</v>
       </c>
       <c r="H22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>33.700000000000045</v>
       </c>
       <c r="I22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.8999999999999773</v>
       </c>
       <c r="J22">
@@ -8297,11 +8298,11 @@
         <v>993</v>
       </c>
       <c r="H23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>22.299999999999955</v>
       </c>
       <c r="I23">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.399999999999977</v>
       </c>
       <c r="J23">
@@ -8331,11 +8332,11 @@
         <v>993.9</v>
       </c>
       <c r="H24">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>30.100000000000023</v>
       </c>
       <c r="I24">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>17.100000000000023</v>
       </c>
       <c r="J24">
@@ -8365,11 +8366,11 @@
         <v>1000.7</v>
       </c>
       <c r="H25">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>42.399999999999977</v>
       </c>
       <c r="I25">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>20.200000000000045</v>
       </c>
       <c r="J25">
@@ -8399,11 +8400,11 @@
         <v>950.5</v>
       </c>
       <c r="H26">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>25.100000000000023</v>
       </c>
       <c r="I26">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>12.700000000000045</v>
       </c>
       <c r="J26">
@@ -8433,11 +8434,11 @@
         <v>1039.2</v>
       </c>
       <c r="H27">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>30</v>
       </c>
       <c r="I27">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
       <c r="J27">
@@ -8467,11 +8468,11 @@
         <v>1017.1</v>
       </c>
       <c r="H28">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>38.400000000000091</v>
       </c>
       <c r="I28">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13.800000000000068</v>
       </c>
       <c r="J28">
@@ -8483,7 +8484,7 @@
         <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C29">
         <v>11</v>
@@ -8501,11 +8502,11 @@
         <v>991.7</v>
       </c>
       <c r="H29">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>24</v>
       </c>
       <c r="I29">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>8.9000000000000909</v>
       </c>
       <c r="J29">
@@ -8517,7 +8518,7 @@
         <v>8</v>
       </c>
       <c r="B30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C30">
         <v>11</v>
@@ -8535,11 +8536,11 @@
         <v>1035.7</v>
       </c>
       <c r="H30">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>21.399999999999864</v>
       </c>
       <c r="I30">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
       <c r="J30">
@@ -8551,7 +8552,7 @@
         <v>8</v>
       </c>
       <c r="B31" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C31">
         <v>12</v>
@@ -8569,11 +8570,11 @@
         <v>1024.8</v>
       </c>
       <c r="H31">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>26.5</v>
       </c>
       <c r="I31">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>9.5999999999999091</v>
       </c>
       <c r="J31">
@@ -8585,7 +8586,7 @@
         <v>8</v>
       </c>
       <c r="B32" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C32">
         <v>12</v>
@@ -8603,11 +8604,11 @@
         <v>988.5</v>
       </c>
       <c r="H32">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>19</v>
       </c>
       <c r="I32">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>6.6000000000000227</v>
       </c>
       <c r="J32">
@@ -8619,7 +8620,7 @@
         <v>8</v>
       </c>
       <c r="B33" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C33">
         <v>12</v>
@@ -8637,11 +8638,11 @@
         <v>947</v>
       </c>
       <c r="H33">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>29.899999999999977</v>
       </c>
       <c r="I33">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>10.799999999999955</v>
       </c>
       <c r="J33">

</xml_diff>